<commit_message>
DB migrated to local
</commit_message>
<xml_diff>
--- a/backend/uploads/Boms.xlsx
+++ b/backend/uploads/Boms.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vedan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A857339-2004-4928-855A-709B16AA4F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FFA96A-4E13-4496-8E8E-600982AA932F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C7201E77-E810-4576-AA06-9C021C48F155}"/>
   </bookViews>
@@ -1068,7 +1068,7 @@
   <dimension ref="A1:H978"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>